<commit_message>
Updated zr25 data from solidworks
</commit_message>
<xml_diff>
--- a/MATLAB/vehicle_data/zr25_data.xlsx
+++ b/MATLAB/vehicle_data/zr25_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bglen/Documents/github/Vehicle-Dynamics/MATLAB/vehicle_zr25/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brian\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA6C903E-04E1-CA4B-9294-1A5868A906E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D322781-9ED4-4B4C-A702-B496F24EA8D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15340" yWindow="500" windowWidth="13460" windowHeight="17220" xr2:uid="{3FBBEF13-1A9E-AE42-92D3-FE7D2663BCC6}"/>
+    <workbookView xWindow="30" yWindow="30" windowWidth="28740" windowHeight="17060" xr2:uid="{3FBBEF13-1A9E-AE42-92D3-FE7D2663BCC6}"/>
   </bookViews>
   <sheets>
     <sheet name="parameters" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="90">
   <si>
     <t>Parameter Name</t>
   </si>
@@ -180,18 +180,9 @@
     <t>kg</t>
   </si>
   <si>
-    <t>percentage on front axle</t>
-  </si>
-  <si>
-    <t>kg * m^2, about the yaw (vertical) axis  of the C.G.</t>
-  </si>
-  <si>
     <t>(# input rotations / # output rotations)</t>
   </si>
   <si>
-    <t>use if tire model not availible</t>
-  </si>
-  <si>
     <t>N/m, from tire data</t>
   </si>
   <si>
@@ -282,20 +273,68 @@
     <t>value needs confirmed</t>
   </si>
   <si>
-    <t>unknown; placeholder value</t>
-  </si>
-  <si>
     <t>track_width_rear</t>
+  </si>
+  <si>
+    <t>roll_polar_inertia</t>
+  </si>
+  <si>
+    <t>pitch_polar_inertia</t>
+  </si>
+  <si>
+    <t>percentage on front axle (0.48, 0.54, 0.54 for drivers ian, dom, abby)</t>
+  </si>
+  <si>
+    <t>kg, from zr25_full</t>
+  </si>
+  <si>
+    <t>m, from zr25_full</t>
+  </si>
+  <si>
+    <t>kg * m^2, about the yaw (vertical, z) axis  of the C.G. from zr25_full</t>
+  </si>
+  <si>
+    <t>kg * m^2, about the roll (longitudinal, x) axis  of the C.G.  from zr25_full</t>
+  </si>
+  <si>
+    <t>kg * m^2, about the pitch (lateral, y) axis  of the C.G.  from zr25_full</t>
+  </si>
+  <si>
+    <t>use if tire model not availible. Typical hot mu vale</t>
+  </si>
+  <si>
+    <t>unknown / placeholder value</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -310,20 +349,17 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -336,16 +372,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="4">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -362,9 +404,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -402,7 +444,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -508,7 +550,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -650,7 +692,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -658,13 +700,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57AD0F8B-F3CF-1548-BE6B-192F596F87AA}">
-  <dimension ref="A1:E53"/>
+  <dimension ref="A1:E55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="42" customWidth="1"/>
     <col min="3" max="3" width="15.83203125" customWidth="1"/>
@@ -672,7 +714,7 @@
     <col min="5" max="5" width="24.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -683,23 +725,23 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C3" s="1" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C3" s="1" t="s">
-        <v>80</v>
-      </c>
       <c r="D3" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -710,7 +752,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -721,9 +763,9 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B6" s="1">
         <v>1.21</v>
@@ -732,18 +774,18 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="2">
-        <v>236.3</v>
+        <v>245.76</v>
       </c>
       <c r="C8" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -754,29 +796,29 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="2">
-        <v>20.48</v>
+        <v>19.818000000000001</v>
       </c>
       <c r="C10" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>8</v>
       </c>
       <c r="B11" s="2">
-        <v>20.48</v>
+        <v>19.818000000000001</v>
       </c>
       <c r="C11" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -784,405 +826,427 @@
         <v>0.48</v>
       </c>
       <c r="C12" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>10</v>
       </c>
       <c r="B13" s="2">
-        <v>0.28000000000000003</v>
+        <v>0.25756000000000001</v>
       </c>
       <c r="C13" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="2">
+        <v>142.91999999999999</v>
+      </c>
+      <c r="C14" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
         <v>80</v>
       </c>
-      <c r="C14" t="s">
+      <c r="B15" s="2">
+        <v>26.46</v>
+      </c>
+      <c r="C15" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>81</v>
+      </c>
+      <c r="B16" s="2">
+        <v>126.29</v>
+      </c>
+      <c r="C16" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C18" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" s="1">
+        <v>11</v>
+      </c>
+      <c r="C19" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" s="3">
+        <v>2</v>
+      </c>
+      <c r="C20" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" s="2">
+        <v>87563.5</v>
+      </c>
+      <c r="C21" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>12</v>
-      </c>
-      <c r="B16" s="1">
-        <v>0.25</v>
-      </c>
-      <c r="C16" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>13</v>
-      </c>
-      <c r="B17" s="3">
-        <v>13</v>
-      </c>
-      <c r="C17" t="s">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22" s="1">
+        <v>0.19</v>
+      </c>
+      <c r="C22" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>17</v>
+      </c>
+      <c r="B24" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C24" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>14</v>
-      </c>
-      <c r="B18" s="3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>18</v>
+      </c>
+      <c r="B25" s="3">
+        <v>0</v>
+      </c>
+      <c r="C25" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>19</v>
+      </c>
+      <c r="B26" s="3">
+        <v>-2.5</v>
+      </c>
+      <c r="C26" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>20</v>
+      </c>
+      <c r="B27" s="3">
+        <v>-2.5</v>
+      </c>
+      <c r="C27" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>21</v>
+      </c>
+      <c r="B28" s="3">
+        <v>7.02</v>
+      </c>
+      <c r="C28" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>22</v>
+      </c>
+      <c r="B29" s="3">
+        <v>70</v>
+      </c>
+      <c r="C29" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>23</v>
+      </c>
+      <c r="B30" s="2">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="C30" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>24</v>
+      </c>
+      <c r="B31" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="C31" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>25</v>
+      </c>
+      <c r="B33" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="C33" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>26</v>
+      </c>
+      <c r="B34" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="C34" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>27</v>
+      </c>
+      <c r="B35" s="3">
         <v>2</v>
       </c>
-      <c r="C18" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>15</v>
-      </c>
-      <c r="B19" s="2">
-        <v>87563.5</v>
-      </c>
-      <c r="C19" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>16</v>
-      </c>
-      <c r="B20" s="1">
-        <v>0.19</v>
-      </c>
-      <c r="C20" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>17</v>
-      </c>
-      <c r="B22" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="C22" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>18</v>
-      </c>
-      <c r="B23" s="3">
-        <v>0</v>
-      </c>
-      <c r="C23" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>19</v>
-      </c>
-      <c r="B24" s="3">
-        <v>-2.5</v>
-      </c>
-      <c r="C24" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>20</v>
-      </c>
-      <c r="B25" s="3">
-        <v>-2.5</v>
-      </c>
-      <c r="C25" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>21</v>
-      </c>
-      <c r="B26" s="3">
-        <v>7.02</v>
-      </c>
-      <c r="C26" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>22</v>
-      </c>
-      <c r="B27" s="3">
-        <v>70</v>
-      </c>
-      <c r="C27" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>23</v>
-      </c>
-      <c r="B28" s="2">
-        <v>3.5000000000000003E-2</v>
-      </c>
-      <c r="C28" t="s">
+      <c r="C35" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>28</v>
+      </c>
+      <c r="B36" s="3">
+        <v>0.45</v>
+      </c>
+      <c r="C36" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>24</v>
-      </c>
-      <c r="B29" s="2">
-        <v>0.05</v>
-      </c>
-      <c r="C29" t="s">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>29</v>
+      </c>
+      <c r="B37" s="1">
+        <v>11.4</v>
+      </c>
+      <c r="C37" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>25</v>
-      </c>
-      <c r="B31" s="3">
-        <v>1.5</v>
-      </c>
-      <c r="C31" t="s">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>30</v>
+      </c>
+      <c r="B38" s="3">
+        <v>2.63</v>
+      </c>
+      <c r="C38" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>26</v>
-      </c>
-      <c r="B32" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="C32" t="s">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>31</v>
+      </c>
+      <c r="B39" s="3">
+        <v>0.45500000000000002</v>
+      </c>
+      <c r="C39" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>32</v>
+      </c>
+      <c r="B40" s="3">
+        <v>31</v>
+      </c>
+      <c r="C40" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>33</v>
+      </c>
+      <c r="B41" s="3">
+        <v>2.59</v>
+      </c>
+      <c r="C41" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>27</v>
-      </c>
-      <c r="B33" s="3">
-        <v>2</v>
-      </c>
-      <c r="C33" t="s">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>34</v>
+      </c>
+      <c r="B42" s="3">
+        <v>0.27600000000000002</v>
+      </c>
+      <c r="C42" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>28</v>
-      </c>
-      <c r="B34" s="3">
-        <v>0.45</v>
-      </c>
-      <c r="C34" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>29</v>
-      </c>
-      <c r="B35" s="1">
-        <v>11.4</v>
-      </c>
-      <c r="C35" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>30</v>
-      </c>
-      <c r="B36" s="3">
-        <v>2.63</v>
-      </c>
-      <c r="C36" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>31</v>
-      </c>
-      <c r="B37" s="3">
-        <v>0.45500000000000002</v>
-      </c>
-      <c r="C37" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>32</v>
-      </c>
-      <c r="B38" s="3">
-        <v>31</v>
-      </c>
-      <c r="C38" t="s">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>35</v>
+      </c>
+      <c r="B44" s="3">
+        <v>5.5E-2</v>
+      </c>
+      <c r="C44" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>33</v>
-      </c>
-      <c r="B39" s="3">
-        <v>2.59</v>
-      </c>
-      <c r="C39" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>34</v>
-      </c>
-      <c r="B40" s="3">
-        <v>0.27600000000000002</v>
-      </c>
-      <c r="C40" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>35</v>
-      </c>
-      <c r="B42" s="3">
-        <v>5.5E-2</v>
-      </c>
-      <c r="C42" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
         <v>36</v>
       </c>
-      <c r="B43" s="2">
+      <c r="B45" s="2">
         <f xml:space="preserve"> 45 * 1000</f>
         <v>45000</v>
       </c>
-      <c r="C43" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
+      <c r="C45" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
         <v>37</v>
       </c>
-      <c r="B44" s="2">
+      <c r="B46" s="2">
         <f xml:space="preserve"> 35 * 1000</f>
         <v>35000</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C46" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>38</v>
+      </c>
+      <c r="B47" s="3">
+        <v>2</v>
+      </c>
+      <c r="C47" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>39</v>
+      </c>
+      <c r="B48" s="3">
+        <v>160.23070000000001</v>
+      </c>
+      <c r="C48" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>40</v>
+      </c>
+      <c r="B49" s="2">
+        <v>1.0009999999999999</v>
+      </c>
+      <c r="C49" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>38</v>
-      </c>
-      <c r="B45" s="3">
-        <v>2</v>
-      </c>
-      <c r="C45" t="s">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>41</v>
+      </c>
+      <c r="B50" s="2">
+        <v>1.006</v>
+      </c>
+      <c r="C50" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>42</v>
+      </c>
+      <c r="B51" s="3">
+        <v>1</v>
+      </c>
+      <c r="C51" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>39</v>
-      </c>
-      <c r="B46" s="3">
-        <v>160.23070000000001</v>
-      </c>
-      <c r="C46" t="s">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>43</v>
+      </c>
+      <c r="B52" s="3">
+        <v>0.158</v>
+      </c>
+      <c r="C52" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>44</v>
+      </c>
+      <c r="B54" s="2">
+        <v>3.4</v>
+      </c>
+      <c r="C54" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>40</v>
-      </c>
-      <c r="B47" s="2">
-        <v>1.0009999999999999</v>
-      </c>
-      <c r="C47" t="s">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>45</v>
+      </c>
+      <c r="B55" s="2">
+        <v>3.7</v>
+      </c>
+      <c r="C55" t="s">
         <v>73</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>41</v>
-      </c>
-      <c r="B48" s="2">
-        <v>1.006</v>
-      </c>
-      <c r="C48" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>42</v>
-      </c>
-      <c r="B49" s="3">
-        <v>1</v>
-      </c>
-      <c r="C49" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>43</v>
-      </c>
-      <c r="B50" s="3">
-        <v>0.158</v>
-      </c>
-      <c r="C50" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
-        <v>44</v>
-      </c>
-      <c r="B52" s="2">
-        <v>3.4</v>
-      </c>
-      <c r="C52" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
-        <v>45</v>
-      </c>
-      <c r="B53" s="2">
-        <v>3.7</v>
-      </c>
-      <c r="C53" t="s">
-        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated vehicle description with steering information
</commit_message>
<xml_diff>
--- a/MATLAB/vehicle_data/zr25_data.xlsx
+++ b/MATLAB/vehicle_data/zr25_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brian\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bglen/Documents/github/Vehicle-Dynamics/MATLAB/vehicle_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D322781-9ED4-4B4C-A702-B496F24EA8D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85FB9105-A380-1149-A28E-05A0617F8EE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="30" windowWidth="28740" windowHeight="17060" xr2:uid="{3FBBEF13-1A9E-AE42-92D3-FE7D2663BCC6}"/>
+    <workbookView xWindow="12600" yWindow="500" windowWidth="15740" windowHeight="17060" xr2:uid="{3FBBEF13-1A9E-AE42-92D3-FE7D2663BCC6}"/>
   </bookViews>
   <sheets>
     <sheet name="parameters" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="100">
   <si>
     <t>Parameter Name</t>
   </si>
@@ -300,17 +300,47 @@
     <t>kg * m^2, about the pitch (lateral, y) axis  of the C.G.  from zr25_full</t>
   </si>
   <si>
-    <t>use if tire model not availible. Typical hot mu vale</t>
-  </si>
-  <si>
     <t>unknown / placeholder value</t>
+  </si>
+  <si>
+    <t>steering_arm_length</t>
+  </si>
+  <si>
+    <t>steering_rack_length</t>
+  </si>
+  <si>
+    <t>steering_rack_to_axis_distance</t>
+  </si>
+  <si>
+    <t>steering_pinion_radius</t>
+  </si>
+  <si>
+    <t>m, perpendicular length between tire rod point and kingpin axis</t>
+  </si>
+  <si>
+    <t>m, eye to eye length of steering rack</t>
+  </si>
+  <si>
+    <t>m, eye to eye length of front tie rod</t>
+  </si>
+  <si>
+    <t>m, distance between kingpin axis and steering rack, parallel to the longitudinal plane of the vehicle</t>
+  </si>
+  <si>
+    <t>m, radius of the steering rack pinion gear (reference for gear ratio calculation)</t>
+  </si>
+  <si>
+    <t>tie_rod_length_front</t>
+  </si>
+  <si>
+    <t>unitless, used if tire model not availible. Typically 2/3 of experimental hot mu vale</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -335,6 +365,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -378,11 +416,12 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -404,9 +443,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -444,7 +483,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -550,7 +589,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -692,7 +731,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -700,13 +739,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57AD0F8B-F3CF-1548-BE6B-192F596F87AA}">
-  <dimension ref="A1:E55"/>
+  <dimension ref="A1:E59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="A64" sqref="A64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="42" customWidth="1"/>
     <col min="3" max="3" width="15.83203125" customWidth="1"/>
@@ -714,23 +753,24 @@
     <col min="5" max="5" width="24.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="4"/>
       <c r="C3" s="1" t="s">
         <v>77</v>
       </c>
@@ -738,10 +778,10 @@
         <v>78</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -752,7 +792,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -763,7 +803,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>79</v>
       </c>
@@ -774,7 +814,10 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="4"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -785,7 +828,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -796,7 +839,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -807,7 +850,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -818,7 +861,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -829,7 +872,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -840,7 +883,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -851,7 +894,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>80</v>
       </c>
@@ -862,7 +905,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>81</v>
       </c>
@@ -873,7 +916,10 @@
         <v>87</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="4"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>12</v>
       </c>
@@ -884,7 +930,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>13</v>
       </c>
@@ -895,18 +941,18 @@
         <v>48</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="3">
+      <c r="B20" s="1">
         <v>2</v>
       </c>
       <c r="C20" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>15</v>
       </c>
@@ -917,7 +963,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>16</v>
       </c>
@@ -928,7 +974,10 @@
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="4"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>17</v>
       </c>
@@ -939,7 +988,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>18</v>
       </c>
@@ -950,7 +999,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>19</v>
       </c>
@@ -961,7 +1010,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>20</v>
       </c>
@@ -972,7 +1021,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>21</v>
       </c>
@@ -983,7 +1032,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>22</v>
       </c>
@@ -994,258 +1043,316 @@
         <v>53</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
+        <v>89</v>
+      </c>
+      <c r="B30" s="2">
+        <v>7.6176178298070302E-2</v>
+      </c>
+      <c r="C30" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>90</v>
+      </c>
+      <c r="B31" s="2">
+        <v>0.38417000000000001</v>
+      </c>
+      <c r="C31" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>98</v>
+      </c>
+      <c r="B32" s="2">
+        <v>0.38704984883732901</v>
+      </c>
+      <c r="C32" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>91</v>
+      </c>
+      <c r="B33" s="2">
+        <v>5.8772999999999999E-2</v>
+      </c>
+      <c r="C33" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>92</v>
+      </c>
+      <c r="B34" s="2">
+        <v>2.29E-2</v>
+      </c>
+      <c r="C34" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
         <v>23</v>
       </c>
-      <c r="B30" s="2">
+      <c r="B35" s="2">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C35" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
         <v>24</v>
       </c>
-      <c r="B31" s="2">
+      <c r="B36" s="2">
         <v>0.05</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C36" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
         <v>25</v>
       </c>
-      <c r="B33" s="3">
+      <c r="B38" s="3">
         <v>1.5</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C38" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
         <v>26</v>
       </c>
-      <c r="B34" s="3">
+      <c r="B39" s="3">
         <v>0.2</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C39" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
         <v>27</v>
       </c>
-      <c r="B35" s="3">
+      <c r="B40" s="3">
         <v>2</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C40" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
         <v>28</v>
       </c>
-      <c r="B36" s="3">
+      <c r="B41" s="3">
         <v>0.45</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C41" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
         <v>29</v>
       </c>
-      <c r="B37" s="1">
+      <c r="B42" s="1">
         <v>11.4</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C42" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
         <v>30</v>
       </c>
-      <c r="B38" s="3">
+      <c r="B43" s="3">
         <v>2.63</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C43" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
         <v>31</v>
       </c>
-      <c r="B39" s="3">
+      <c r="B44" s="3">
         <v>0.45500000000000002</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C44" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
         <v>32</v>
       </c>
-      <c r="B40" s="3">
+      <c r="B45" s="3">
         <v>31</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C45" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
         <v>33</v>
       </c>
-      <c r="B41" s="3">
+      <c r="B46" s="3">
         <v>2.59</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C46" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
         <v>34</v>
       </c>
-      <c r="B42" s="3">
+      <c r="B47" s="3">
         <v>0.27600000000000002</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C47" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" s="4"/>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
         <v>35</v>
       </c>
-      <c r="B44" s="3">
+      <c r="B49" s="3">
         <v>5.5E-2</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C49" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A45" t="s">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
         <v>36</v>
       </c>
-      <c r="B45" s="2">
+      <c r="B50" s="2">
         <f xml:space="preserve"> 45 * 1000</f>
         <v>45000</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C50" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A46" t="s">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
         <v>37</v>
       </c>
-      <c r="B46" s="2">
+      <c r="B51" s="2">
         <f xml:space="preserve"> 35 * 1000</f>
         <v>35000</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C51" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A47" t="s">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
         <v>38</v>
       </c>
-      <c r="B47" s="3">
+      <c r="B52" s="3">
         <v>2</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C52" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A48" t="s">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
         <v>39</v>
       </c>
-      <c r="B48" s="3">
+      <c r="B53" s="3">
         <v>160.23070000000001</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C53" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A49" t="s">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
         <v>40</v>
       </c>
-      <c r="B49" s="2">
+      <c r="B54" s="2">
         <v>1.0009999999999999</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C54" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A50" t="s">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
         <v>41</v>
       </c>
-      <c r="B50" s="2">
+      <c r="B55" s="2">
         <v>1.006</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C55" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A51" t="s">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
         <v>42</v>
       </c>
-      <c r="B51" s="3">
+      <c r="B56" s="3">
         <v>1</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C56" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A52" t="s">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
         <v>43</v>
       </c>
-      <c r="B52" s="3">
+      <c r="B57" s="3">
         <v>0.158</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C57" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A54" t="s">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
         <v>44</v>
       </c>
-      <c r="B54" s="2">
+      <c r="B58" s="2">
         <v>3.4</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C58" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A55" t="s">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
         <v>45</v>
       </c>
-      <c r="B55" s="2">
+      <c r="B59" s="2">
         <v>3.7</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C59" t="s">
         <v>73</v>
       </c>
     </row>

</xml_diff>

<commit_message>
compliance in vehicle data model
</commit_message>
<xml_diff>
--- a/MATLAB/vehicle_data/zr25_data.xlsx
+++ b/MATLAB/vehicle_data/zr25_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bglen/Documents/github/Vehicle-Dynamics/MATLAB/vehicle_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD690253-09D5-2B49-8B8B-1BF52F15883A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55583D1E-FAAF-F140-9F49-03D9D0C70EF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13140" yWindow="500" windowWidth="15480" windowHeight="17060" xr2:uid="{3FBBEF13-1A9E-AE42-92D3-FE7D2663BCC6}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="104">
   <si>
     <t>Parameter Name</t>
   </si>
@@ -333,13 +333,19 @@
     <t>tie_rod_length_front</t>
   </si>
   <si>
-    <t>unitless, used if tire model not availible. Typically 2/3 of experimental hot mu vale</t>
-  </si>
-  <si>
     <t>tire_mu_correction_factor</t>
   </si>
   <si>
-    <t>use with tire data to linearly adjust mu values to adjust belt friction to road friction, based on experimental testing</t>
+    <t>unitless, used if nonlinear tire model not availible. Typically 2/3 of experimental hot mu vale</t>
+  </si>
+  <si>
+    <t>use with tire data to linearly adjust mu values to adjust belt friction to road friction, based on experimental testing (const radius test)</t>
+  </si>
+  <si>
+    <t>deg per 1kN, per wheel, toe deflection from Fy forces, from experimental testing</t>
+  </si>
+  <si>
+    <t>toe_deflection_from_rear</t>
   </si>
 </sst>
 </file>
@@ -745,10 +751,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57AD0F8B-F3CF-1548-BE6B-192F596F87AA}">
-  <dimension ref="A1:E60"/>
+  <dimension ref="A1:E62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="A62" sqref="A62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -955,14 +961,14 @@
         <v>2</v>
       </c>
       <c r="C20" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>100</v>
-      </c>
-      <c r="B21" s="1">
+        <v>99</v>
+      </c>
+      <c r="B21" s="3">
         <v>0.66</v>
       </c>
       <c r="C21" t="s">
@@ -1371,6 +1377,17 @@
       </c>
       <c r="C60" t="s">
         <v>73</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>103</v>
+      </c>
+      <c r="B62" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="C62" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed load transfer bug
Updated vehicle mass; fixed load transfer calc that over-calculated load transfer. It now matches the expected lateral G's to cause a rollover.
</commit_message>
<xml_diff>
--- a/MATLAB/vehicle_data/zr25_data.xlsx
+++ b/MATLAB/vehicle_data/zr25_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bglen/Documents/github/Vehicle-Dynamics/MATLAB/vehicle_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2866E1FE-042E-D241-9CDB-791BA483BDB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BBE0D1C-35D3-4245-AEDE-C8C673BF49B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13140" yWindow="500" windowWidth="15480" windowHeight="17060" xr2:uid="{3FBBEF13-1A9E-AE42-92D3-FE7D2663BCC6}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="13080" windowHeight="17500" xr2:uid="{3FBBEF13-1A9E-AE42-92D3-FE7D2663BCC6}"/>
   </bookViews>
   <sheets>
     <sheet name="parameters" sheetId="1" r:id="rId1"/>
@@ -753,13 +753,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57AD0F8B-F3CF-1548-BE6B-192F596F87AA}">
   <dimension ref="A1:E62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="A62" sqref="A62"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="42" customWidth="1"/>
+    <col min="1" max="1" width="33.5" customWidth="1"/>
     <col min="3" max="3" width="15.83203125" customWidth="1"/>
     <col min="4" max="4" width="20.83203125" customWidth="1"/>
     <col min="5" max="5" width="24.33203125" customWidth="1"/>
@@ -834,7 +834,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="2">
-        <v>245.76</v>
+        <v>225.91499999999999</v>
       </c>
       <c r="C8" t="s">
         <v>83</v>
@@ -856,7 +856,7 @@
         <v>7</v>
       </c>
       <c r="B10" s="2">
-        <v>19.818000000000001</v>
+        <v>18.31025</v>
       </c>
       <c r="C10" t="s">
         <v>75</v>
@@ -867,7 +867,7 @@
         <v>8</v>
       </c>
       <c r="B11" s="2">
-        <v>19.818000000000001</v>
+        <v>18.31025</v>
       </c>
       <c r="C11" t="s">
         <v>75</v>

</xml_diff>

<commit_message>
Updated vehicle model to include tire mu correction factor
used by reference generation to modify maximum acceleration limits based on the track conditions
</commit_message>
<xml_diff>
--- a/MATLAB/vehicle_data/zr25_data.xlsx
+++ b/MATLAB/vehicle_data/zr25_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bglen/Documents/github/Vehicle-Dynamics/MATLAB/vehicle_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BBE0D1C-35D3-4245-AEDE-C8C673BF49B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F713BC13-8251-A242-826B-4884678AD96D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="13080" windowHeight="17500" xr2:uid="{3FBBEF13-1A9E-AE42-92D3-FE7D2663BCC6}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23080" windowHeight="17500" xr2:uid="{3FBBEF13-1A9E-AE42-92D3-FE7D2663BCC6}"/>
   </bookViews>
   <sheets>
     <sheet name="parameters" sheetId="1" r:id="rId1"/>
@@ -34,10 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="104">
-  <si>
-    <t>Parameter Name</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="112">
   <si>
     <t>Value</t>
   </si>
@@ -346,6 +343,33 @@
   </si>
   <si>
     <t>toe_deflection_rear</t>
+  </si>
+  <si>
+    <t>Parameter</t>
+  </si>
+  <si>
+    <t>motor_inertia</t>
+  </si>
+  <si>
+    <t>electric motor rotational inertia</t>
+  </si>
+  <si>
+    <t>gearbox_inertia</t>
+  </si>
+  <si>
+    <t>inertia of gearbox components as seen by the input shaft</t>
+  </si>
+  <si>
+    <t>output_shaft_inertia</t>
+  </si>
+  <si>
+    <t>inertia of ouput shaft components not included in gearbox_inertia (hub, brake rotor, lug nuts, etc)</t>
+  </si>
+  <si>
+    <t>wheel_inertia</t>
+  </si>
+  <si>
+    <t>inertia of rim and tire</t>
   </si>
 </sst>
 </file>
@@ -751,10 +775,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57AD0F8B-F3CF-1548-BE6B-192F596F87AA}">
-  <dimension ref="A1:E62"/>
+  <dimension ref="A1:E67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -767,63 +791,63 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="4"/>
       <c r="C3" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>78</v>
-      </c>
       <c r="E3" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="1">
         <v>1.53</v>
       </c>
       <c r="C4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="1">
         <v>1.23</v>
       </c>
       <c r="C5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B6" s="1">
         <v>1.21</v>
       </c>
       <c r="C6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -831,101 +855,101 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8" s="2">
         <v>225.91499999999999</v>
       </c>
       <c r="C8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9" s="1">
         <v>72.73</v>
       </c>
       <c r="C9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10" s="2">
         <v>18.31025</v>
       </c>
       <c r="C10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B11" s="2">
         <v>18.31025</v>
       </c>
       <c r="C11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B12" s="2">
         <v>0.48</v>
       </c>
       <c r="C12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B13" s="2">
         <v>0.25756000000000001</v>
       </c>
       <c r="C13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B14" s="2">
         <v>142.91999999999999</v>
       </c>
       <c r="C14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B15" s="2">
         <v>26.46</v>
       </c>
       <c r="C15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B16" s="2">
         <v>126.29</v>
       </c>
       <c r="C16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -933,13 +957,13 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B18" s="1">
         <v>0.25</v>
       </c>
       <c r="C18" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -947,18 +971,18 @@
         <v>13</v>
       </c>
       <c r="B19" s="1">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C19" t="s">
-        <v>48</v>
+        <v>99</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>14</v>
-      </c>
-      <c r="B20" s="1">
-        <v>2</v>
+        <v>98</v>
+      </c>
+      <c r="B20" s="3">
+        <v>0.66</v>
       </c>
       <c r="C20" t="s">
         <v>100</v>
@@ -966,255 +990,244 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>99</v>
-      </c>
-      <c r="B21" s="3">
-        <v>0.66</v>
+        <v>14</v>
+      </c>
+      <c r="B21" s="2">
+        <v>87563.5</v>
       </c>
       <c r="C21" t="s">
-        <v>101</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>15</v>
       </c>
-      <c r="B22" s="2">
-        <v>87563.5</v>
+      <c r="B22" s="1">
+        <v>0.19</v>
       </c>
       <c r="C22" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>16</v>
-      </c>
-      <c r="B23" s="1">
-        <v>0.19</v>
-      </c>
-      <c r="C23" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="4"/>
+      <c r="A24" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24" s="1">
+        <v>11</v>
+      </c>
+      <c r="C24" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>17</v>
-      </c>
-      <c r="B25" s="3">
-        <v>0.5</v>
+        <v>104</v>
+      </c>
+      <c r="B25" s="1">
+        <v>2.7399999999999999E-4</v>
       </c>
       <c r="C25" t="s">
-        <v>50</v>
+        <v>105</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>18</v>
+        <v>106</v>
       </c>
       <c r="B26" s="3">
-        <v>0</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="C26" t="s">
-        <v>50</v>
+        <v>107</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>19</v>
+        <v>108</v>
       </c>
       <c r="B27" s="3">
-        <v>-2.5</v>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="C27" t="s">
-        <v>51</v>
+        <v>109</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>20</v>
+        <v>110</v>
       </c>
       <c r="B28" s="3">
-        <v>-2.5</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="C28" t="s">
-        <v>51</v>
+        <v>111</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>21</v>
-      </c>
-      <c r="B29" s="3">
-        <v>7.02</v>
-      </c>
-      <c r="C29" t="s">
-        <v>52</v>
-      </c>
+      <c r="A29" s="4"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B30" s="3">
-        <v>70</v>
+        <v>0.5</v>
       </c>
       <c r="C30" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>89</v>
-      </c>
-      <c r="B31" s="2">
-        <v>7.6176178298070302E-2</v>
+        <v>17</v>
+      </c>
+      <c r="B31" s="3">
+        <v>0</v>
       </c>
       <c r="C31" t="s">
-        <v>93</v>
+        <v>49</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>90</v>
-      </c>
-      <c r="B32" s="2">
-        <v>0.38417000000000001</v>
+        <v>18</v>
+      </c>
+      <c r="B32" s="3">
+        <v>-2.5</v>
       </c>
       <c r="C32" t="s">
-        <v>94</v>
+        <v>50</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>98</v>
-      </c>
-      <c r="B33" s="2">
-        <v>0.38704984883732901</v>
+        <v>19</v>
+      </c>
+      <c r="B33" s="3">
+        <v>-2.5</v>
       </c>
       <c r="C33" t="s">
-        <v>95</v>
+        <v>50</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>91</v>
-      </c>
-      <c r="B34" s="2">
-        <v>5.8772999999999999E-2</v>
+        <v>20</v>
+      </c>
+      <c r="B34" s="3">
+        <v>7.02</v>
       </c>
       <c r="C34" t="s">
-        <v>96</v>
+        <v>51</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>92</v>
-      </c>
-      <c r="B35" s="2">
-        <v>2.29E-2</v>
+        <v>21</v>
+      </c>
+      <c r="B35" s="3">
+        <v>70</v>
       </c>
       <c r="C35" t="s">
-        <v>97</v>
+        <v>52</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>23</v>
+        <v>88</v>
       </c>
       <c r="B36" s="2">
-        <v>3.5000000000000003E-2</v>
+        <v>7.6176178298070302E-2</v>
       </c>
       <c r="C36" t="s">
-        <v>54</v>
+        <v>92</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>24</v>
+        <v>89</v>
       </c>
       <c r="B37" s="2">
-        <v>0.05</v>
+        <v>0.38417000000000001</v>
       </c>
       <c r="C37" t="s">
-        <v>55</v>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>97</v>
+      </c>
+      <c r="B38" s="2">
+        <v>0.38704984883732901</v>
+      </c>
+      <c r="C38" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>25</v>
-      </c>
-      <c r="B39" s="3">
-        <v>1.5</v>
+        <v>90</v>
+      </c>
+      <c r="B39" s="2">
+        <v>5.8772999999999999E-2</v>
       </c>
       <c r="C39" t="s">
-        <v>56</v>
+        <v>95</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>26</v>
-      </c>
-      <c r="B40" s="3">
-        <v>0.2</v>
+        <v>91</v>
+      </c>
+      <c r="B40" s="2">
+        <v>2.29E-2</v>
       </c>
       <c r="C40" t="s">
-        <v>61</v>
+        <v>96</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>27</v>
-      </c>
-      <c r="B41" s="3">
-        <v>2</v>
+        <v>22</v>
+      </c>
+      <c r="B41" s="2">
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="C41" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>28</v>
-      </c>
-      <c r="B42" s="3">
-        <v>0.45</v>
+        <v>23</v>
+      </c>
+      <c r="B42" s="2">
+        <v>0.05</v>
       </c>
       <c r="C42" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>29</v>
-      </c>
-      <c r="B43" s="1">
-        <v>11.4</v>
-      </c>
-      <c r="C43" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B44" s="3">
-        <v>2.63</v>
+        <v>1.5</v>
       </c>
       <c r="C44" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B45" s="3">
-        <v>0.45500000000000002</v>
+        <v>0.2</v>
       </c>
       <c r="C45" t="s">
         <v>60</v>
@@ -1222,172 +1235,227 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B46" s="3">
-        <v>31</v>
+        <v>2</v>
       </c>
       <c r="C46" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B47" s="3">
-        <v>2.59</v>
+        <v>0.45</v>
       </c>
       <c r="C47" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>34</v>
-      </c>
-      <c r="B48" s="3">
-        <v>0.27600000000000002</v>
+        <v>28</v>
+      </c>
+      <c r="B48" s="1">
+        <v>11.4</v>
       </c>
       <c r="C48" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A49" s="4"/>
+      <c r="A49" t="s">
+        <v>29</v>
+      </c>
+      <c r="B49" s="3">
+        <v>2.63</v>
+      </c>
+      <c r="C49" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B50" s="3">
-        <v>5.5E-2</v>
+        <v>0.45500000000000002</v>
       </c>
       <c r="C50" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>36</v>
-      </c>
-      <c r="B51" s="2">
+        <v>31</v>
+      </c>
+      <c r="B51" s="3">
+        <v>31</v>
+      </c>
+      <c r="C51" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>32</v>
+      </c>
+      <c r="B52" s="3">
+        <v>2.59</v>
+      </c>
+      <c r="C52" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>33</v>
+      </c>
+      <c r="B53" s="3">
+        <v>0.27600000000000002</v>
+      </c>
+      <c r="C53" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" s="4"/>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>34</v>
+      </c>
+      <c r="B55" s="3">
+        <v>5.5E-2</v>
+      </c>
+      <c r="C55" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>35</v>
+      </c>
+      <c r="B56" s="2">
         <f xml:space="preserve"> 45 * 1000</f>
         <v>45000</v>
       </c>
-      <c r="C51" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
-        <v>37</v>
-      </c>
-      <c r="B52" s="2">
+      <c r="C56" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>36</v>
+      </c>
+      <c r="B57" s="2">
         <f xml:space="preserve"> 35 * 1000</f>
         <v>35000</v>
       </c>
-      <c r="C52" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
-        <v>38</v>
-      </c>
-      <c r="B53" s="3">
-        <v>2</v>
-      </c>
-      <c r="C53" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
-        <v>39</v>
-      </c>
-      <c r="B54" s="3">
-        <v>160.23070000000001</v>
-      </c>
-      <c r="C54" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
-        <v>40</v>
-      </c>
-      <c r="B55" s="2">
-        <v>1.0009999999999999</v>
-      </c>
-      <c r="C55" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
-        <v>41</v>
-      </c>
-      <c r="B56" s="2">
-        <v>1.006</v>
-      </c>
-      <c r="C56" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
-        <v>42</v>
-      </c>
-      <c r="B57" s="3">
-        <v>1</v>
-      </c>
       <c r="C57" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B58" s="3">
-        <v>0.158</v>
+        <v>2</v>
       </c>
       <c r="C58" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>44</v>
-      </c>
-      <c r="B59" s="2">
-        <v>3.4</v>
+        <v>38</v>
+      </c>
+      <c r="B59" s="3">
+        <v>160.23070000000001</v>
       </c>
       <c r="C59" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B60" s="2">
-        <v>3.7</v>
+        <v>1.0009999999999999</v>
       </c>
       <c r="C60" t="s">
-        <v>73</v>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>40</v>
+      </c>
+      <c r="B61" s="2">
+        <v>1.006</v>
+      </c>
+      <c r="C61" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>103</v>
-      </c>
-      <c r="B62" s="2">
+        <v>41</v>
+      </c>
+      <c r="B62" s="3">
+        <v>1</v>
+      </c>
+      <c r="C62" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>42</v>
+      </c>
+      <c r="B63" s="3">
+        <v>0.158</v>
+      </c>
+      <c r="C63" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>43</v>
+      </c>
+      <c r="B64" s="2">
+        <v>3.4</v>
+      </c>
+      <c r="C64" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>44</v>
+      </c>
+      <c r="B65" s="2">
+        <v>3.7</v>
+      </c>
+      <c r="C65" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>102</v>
+      </c>
+      <c r="B67" s="2">
         <v>0.1</v>
       </c>
-      <c r="C62" t="s">
-        <v>102</v>
+      <c r="C67" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated vehicle data to include gearbox parameters
</commit_message>
<xml_diff>
--- a/MATLAB/vehicle_data/zr25_data.xlsx
+++ b/MATLAB/vehicle_data/zr25_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bglen/Documents/github/Vehicle-Dynamics/MATLAB/vehicle_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F713BC13-8251-A242-826B-4884678AD96D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD9B4420-1091-AC4B-AF6B-374611593B54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="23080" windowHeight="17500" xr2:uid="{3FBBEF13-1A9E-AE42-92D3-FE7D2663BCC6}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="16020" windowHeight="17500" xr2:uid="{3FBBEF13-1A9E-AE42-92D3-FE7D2663BCC6}"/>
   </bookViews>
   <sheets>
     <sheet name="parameters" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="116">
   <si>
     <t>Value</t>
   </si>
@@ -348,28 +348,40 @@
     <t>Parameter</t>
   </si>
   <si>
-    <t>motor_inertia</t>
-  </si>
-  <si>
     <t>electric motor rotational inertia</t>
   </si>
   <si>
-    <t>gearbox_inertia</t>
-  </si>
-  <si>
     <t>inertia of gearbox components as seen by the input shaft</t>
   </si>
   <si>
-    <t>output_shaft_inertia</t>
-  </si>
-  <si>
     <t>inertia of ouput shaft components not included in gearbox_inertia (hub, brake rotor, lug nuts, etc)</t>
   </si>
   <si>
-    <t>wheel_inertia</t>
-  </si>
-  <si>
     <t>inertia of rim and tire</t>
+  </si>
+  <si>
+    <t>j_m</t>
+  </si>
+  <si>
+    <t>J_s1</t>
+  </si>
+  <si>
+    <t>J_1</t>
+  </si>
+  <si>
+    <t>J_2</t>
+  </si>
+  <si>
+    <t>J_s2</t>
+  </si>
+  <si>
+    <t>J_w</t>
+  </si>
+  <si>
+    <t>inertia of gearbox input shaft (motor is the input shaft so this is zero)</t>
+  </si>
+  <si>
+    <t>inertia of gearbox components as seen by the output shaft (using J_1 so this must be zero)</t>
   </si>
 </sst>
 </file>
@@ -775,10 +787,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57AD0F8B-F3CF-1548-BE6B-192F596F87AA}">
-  <dimension ref="A1:E67"/>
+  <dimension ref="A1:E69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1014,8 +1026,8 @@
       <c r="A24" t="s">
         <v>12</v>
       </c>
-      <c r="B24" s="1">
-        <v>11</v>
+      <c r="B24" s="2">
+        <v>12</v>
       </c>
       <c r="C24" t="s">
         <v>47</v>
@@ -1023,438 +1035,460 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="B25" s="1">
         <v>2.7399999999999999E-4</v>
       </c>
       <c r="C25" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="B26" s="3">
-        <v>8.0000000000000004E-4</v>
+        <v>0</v>
       </c>
       <c r="C26" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B27" s="3">
-        <v>5.0000000000000001E-4</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="C27" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B28" s="3">
-        <v>3.0000000000000001E-3</v>
+        <v>0</v>
       </c>
       <c r="C28" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" s="4"/>
+      <c r="A29" t="s">
+        <v>112</v>
+      </c>
+      <c r="B29" s="3">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="C29" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>16</v>
+        <v>113</v>
       </c>
       <c r="B30" s="3">
-        <v>0.5</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="C30" t="s">
-        <v>49</v>
+        <v>107</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>17</v>
-      </c>
-      <c r="B31" s="3">
-        <v>0</v>
-      </c>
-      <c r="C31" t="s">
-        <v>49</v>
-      </c>
+      <c r="A31" s="4"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B32" s="3">
-        <v>-2.5</v>
+        <v>0.5</v>
       </c>
       <c r="C32" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B33" s="3">
-        <v>-2.5</v>
+        <v>0</v>
       </c>
       <c r="C33" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B34" s="3">
-        <v>7.02</v>
+        <v>-2.5</v>
       </c>
       <c r="C34" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B35" s="3">
-        <v>70</v>
+        <v>-2.5</v>
       </c>
       <c r="C35" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>88</v>
-      </c>
-      <c r="B36" s="2">
-        <v>7.6176178298070302E-2</v>
+        <v>20</v>
+      </c>
+      <c r="B36" s="3">
+        <v>7.02</v>
       </c>
       <c r="C36" t="s">
-        <v>92</v>
+        <v>51</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>89</v>
-      </c>
-      <c r="B37" s="2">
-        <v>0.38417000000000001</v>
+        <v>21</v>
+      </c>
+      <c r="B37" s="3">
+        <v>70</v>
       </c>
       <c r="C37" t="s">
-        <v>93</v>
+        <v>52</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="B38" s="2">
-        <v>0.38704984883732901</v>
+        <v>7.6176178298070302E-2</v>
       </c>
       <c r="C38" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B39" s="2">
-        <v>5.8772999999999999E-2</v>
+        <v>0.38417000000000001</v>
       </c>
       <c r="C39" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="B40" s="2">
-        <v>2.29E-2</v>
+        <v>0.38704984883732901</v>
       </c>
       <c r="C40" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>22</v>
+        <v>90</v>
       </c>
       <c r="B41" s="2">
-        <v>3.5000000000000003E-2</v>
+        <v>5.8772999999999999E-2</v>
       </c>
       <c r="C41" t="s">
-        <v>53</v>
+        <v>95</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>23</v>
+        <v>91</v>
       </c>
       <c r="B42" s="2">
-        <v>0.05</v>
+        <v>2.29E-2</v>
       </c>
       <c r="C42" t="s">
-        <v>54</v>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>22</v>
+      </c>
+      <c r="B43" s="2">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="C43" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>24</v>
-      </c>
-      <c r="B44" s="3">
-        <v>1.5</v>
+        <v>23</v>
+      </c>
+      <c r="B44" s="2">
+        <v>0.05</v>
       </c>
       <c r="C44" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>25</v>
-      </c>
-      <c r="B45" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="C45" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B46" s="3">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="C46" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B47" s="3">
-        <v>0.45</v>
+        <v>0.2</v>
       </c>
       <c r="C47" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>28</v>
-      </c>
-      <c r="B48" s="1">
-        <v>11.4</v>
+        <v>26</v>
+      </c>
+      <c r="B48" s="3">
+        <v>2</v>
       </c>
       <c r="C48" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B49" s="3">
-        <v>2.63</v>
+        <v>0.45</v>
       </c>
       <c r="C49" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>30</v>
-      </c>
-      <c r="B50" s="3">
-        <v>0.45500000000000002</v>
+        <v>28</v>
+      </c>
+      <c r="B50" s="1">
+        <v>11.4</v>
       </c>
       <c r="C50" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B51" s="3">
-        <v>31</v>
+        <v>2.63</v>
       </c>
       <c r="C51" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B52" s="3">
-        <v>2.59</v>
+        <v>0.45500000000000002</v>
       </c>
       <c r="C52" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B53" s="3">
-        <v>0.27600000000000002</v>
+        <v>31</v>
       </c>
       <c r="C53" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A54" s="4"/>
+      <c r="A54" t="s">
+        <v>32</v>
+      </c>
+      <c r="B54" s="3">
+        <v>2.59</v>
+      </c>
+      <c r="C54" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
+        <v>33</v>
+      </c>
+      <c r="B55" s="3">
+        <v>0.27600000000000002</v>
+      </c>
+      <c r="C55" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" s="4"/>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
         <v>34</v>
       </c>
-      <c r="B55" s="3">
+      <c r="B57" s="3">
         <v>5.5E-2</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C57" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
         <v>35</v>
       </c>
-      <c r="B56" s="2">
+      <c r="B58" s="2">
         <f xml:space="preserve"> 45 * 1000</f>
         <v>45000</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C58" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
         <v>36</v>
       </c>
-      <c r="B57" s="2">
+      <c r="B59" s="2">
         <f xml:space="preserve"> 35 * 1000</f>
         <v>35000</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C59" t="s">
         <v>66</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
-        <v>37</v>
-      </c>
-      <c r="B58" s="3">
-        <v>2</v>
-      </c>
-      <c r="C58" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
-        <v>38</v>
-      </c>
-      <c r="B59" s="3">
-        <v>160.23070000000001</v>
-      </c>
-      <c r="C59" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>39</v>
-      </c>
-      <c r="B60" s="2">
-        <v>1.0009999999999999</v>
+        <v>37</v>
+      </c>
+      <c r="B60" s="3">
+        <v>2</v>
       </c>
       <c r="C60" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>40</v>
-      </c>
-      <c r="B61" s="2">
-        <v>1.006</v>
+        <v>38</v>
+      </c>
+      <c r="B61" s="3">
+        <v>160.23070000000001</v>
       </c>
       <c r="C61" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>41</v>
-      </c>
-      <c r="B62" s="3">
-        <v>1</v>
+        <v>39</v>
+      </c>
+      <c r="B62" s="2">
+        <v>1.0009999999999999</v>
       </c>
       <c r="C62" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>42</v>
-      </c>
-      <c r="B63" s="3">
-        <v>0.158</v>
+        <v>40</v>
+      </c>
+      <c r="B63" s="2">
+        <v>1.006</v>
       </c>
       <c r="C63" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>43</v>
-      </c>
-      <c r="B64" s="2">
-        <v>3.4</v>
+        <v>41</v>
+      </c>
+      <c r="B64" s="3">
+        <v>1</v>
       </c>
       <c r="C64" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>44</v>
-      </c>
-      <c r="B65" s="2">
-        <v>3.7</v>
+        <v>42</v>
+      </c>
+      <c r="B65" s="3">
+        <v>0.158</v>
       </c>
       <c r="C65" t="s">
-        <v>72</v>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>43</v>
+      </c>
+      <c r="B66" s="2">
+        <v>3.4</v>
+      </c>
+      <c r="C66" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
+        <v>44</v>
+      </c>
+      <c r="B67" s="2">
+        <v>3.7</v>
+      </c>
+      <c r="C67" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
         <v>102</v>
       </c>
-      <c r="B67" s="2">
+      <c r="B69" s="2">
         <v>0.1</v>
       </c>
-      <c r="C67" t="s">
+      <c r="C69" t="s">
         <v>101</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated vehicle design sheet to include brake parameters
</commit_message>
<xml_diff>
--- a/MATLAB/vehicle_data/zr25_data.xlsx
+++ b/MATLAB/vehicle_data/zr25_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bglen/Documents/github/Vehicle-Dynamics/MATLAB/vehicle_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD9B4420-1091-AC4B-AF6B-374611593B54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2B0D03A-48A4-9D43-B7D6-0BD633835B14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="16020" windowHeight="17500" xr2:uid="{3FBBEF13-1A9E-AE42-92D3-FE7D2663BCC6}"/>
+    <workbookView xWindow="60" yWindow="500" windowWidth="14240" windowHeight="17500" xr2:uid="{3FBBEF13-1A9E-AE42-92D3-FE7D2663BCC6}"/>
   </bookViews>
   <sheets>
     <sheet name="parameters" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="138">
   <si>
     <t>Value</t>
   </si>
@@ -382,6 +382,72 @@
   </si>
   <si>
     <t>inertia of gearbox components as seen by the output shaft (using J_1 so this must be zero)</t>
+  </si>
+  <si>
+    <t>piston_radius_front</t>
+  </si>
+  <si>
+    <t>piston_radius_rear</t>
+  </si>
+  <si>
+    <t>num_pistons_rear</t>
+  </si>
+  <si>
+    <t>pad_friction_front</t>
+  </si>
+  <si>
+    <t>pad_friction_rear</t>
+  </si>
+  <si>
+    <t>max_pedal_force</t>
+  </si>
+  <si>
+    <t>unitless</t>
+  </si>
+  <si>
+    <t>disc_radius_front</t>
+  </si>
+  <si>
+    <t>disc_radius_rear</t>
+  </si>
+  <si>
+    <t>pad_height_front</t>
+  </si>
+  <si>
+    <t>pad_height_rear</t>
+  </si>
+  <si>
+    <t>num_pistons_front</t>
+  </si>
+  <si>
+    <t>m, 0.5 in</t>
+  </si>
+  <si>
+    <t>N, 150 lbf</t>
+  </si>
+  <si>
+    <t>mc_diameter_front</t>
+  </si>
+  <si>
+    <t>mc_diameter_rear</t>
+  </si>
+  <si>
+    <t>balance_bar_ratio_front</t>
+  </si>
+  <si>
+    <t>m, 0.625 in</t>
+  </si>
+  <si>
+    <t>m, 0.9375 in</t>
+  </si>
+  <si>
+    <t>m, 1 in</t>
+  </si>
+  <si>
+    <t>m, 5.125 in</t>
+  </si>
+  <si>
+    <t>0 to 1, from brake design spreadsheet</t>
   </si>
 </sst>
 </file>
@@ -787,10 +853,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57AD0F8B-F3CF-1548-BE6B-192F596F87AA}">
-  <dimension ref="A1:E69"/>
+  <dimension ref="A1:E84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="D78" sqref="D78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1492,7 +1558,162 @@
         <v>101</v>
       </c>
     </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>116</v>
+      </c>
+      <c r="B71" s="2">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="C71" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>117</v>
+      </c>
+      <c r="B72" s="2">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="C72" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>127</v>
+      </c>
+      <c r="B73" s="2">
+        <v>2</v>
+      </c>
+      <c r="C73" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>118</v>
+      </c>
+      <c r="B74" s="2">
+        <v>2</v>
+      </c>
+      <c r="C74" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>119</v>
+      </c>
+      <c r="B75" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="C75" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>120</v>
+      </c>
+      <c r="B76" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="C76" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>121</v>
+      </c>
+      <c r="B77" s="2">
+        <v>667.23</v>
+      </c>
+      <c r="C77" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>123</v>
+      </c>
+      <c r="B78" s="2">
+        <v>0.13</v>
+      </c>
+      <c r="C78" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>124</v>
+      </c>
+      <c r="B79" s="2">
+        <v>0.13</v>
+      </c>
+      <c r="C79" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>125</v>
+      </c>
+      <c r="B80" s="2">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="C80" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>126</v>
+      </c>
+      <c r="B81" s="2">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="C81" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>130</v>
+      </c>
+      <c r="B82" s="2">
+        <v>1.6E-2</v>
+      </c>
+      <c r="C82" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>131</v>
+      </c>
+      <c r="B83" s="2">
+        <v>2.4E-2</v>
+      </c>
+      <c r="C83" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>132</v>
+      </c>
+      <c r="B84" s="2">
+        <v>0.51519999999999999</v>
+      </c>
+      <c r="C84" t="s">
+        <v>137</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Mechanical braking system in model
Used to determine regen limits based on applied brake pressure.
</commit_message>
<xml_diff>
--- a/MATLAB/vehicle_data/zr25_data.xlsx
+++ b/MATLAB/vehicle_data/zr25_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bglen/Documents/github/Vehicle-Dynamics/MATLAB/vehicle_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2B0D03A-48A4-9D43-B7D6-0BD633835B14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1D509F9-E984-A344-98F3-05487CDDD2B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="500" windowWidth="14240" windowHeight="17500" xr2:uid="{3FBBEF13-1A9E-AE42-92D3-FE7D2663BCC6}"/>
+    <workbookView xWindow="960" yWindow="500" windowWidth="16460" windowHeight="17500" xr2:uid="{3FBBEF13-1A9E-AE42-92D3-FE7D2663BCC6}"/>
   </bookViews>
   <sheets>
     <sheet name="parameters" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="139">
   <si>
     <t>Value</t>
   </si>
@@ -448,6 +448,9 @@
   </si>
   <si>
     <t>0 to 1, from brake design spreadsheet</t>
+  </si>
+  <si>
+    <t>brake_pedal_motion_ratio</t>
   </si>
 </sst>
 </file>
@@ -853,10 +856,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57AD0F8B-F3CF-1548-BE6B-192F596F87AA}">
-  <dimension ref="A1:E84"/>
+  <dimension ref="A1:E85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="D78" sqref="D78"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="D87" sqref="D87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1712,6 +1715,17 @@
         <v>137</v>
       </c>
     </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>138</v>
+      </c>
+      <c r="B85" s="2">
+        <v>3.77</v>
+      </c>
+      <c r="C85" t="s">
+        <v>122</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Added more drivetrain parameters to vehicle model
</commit_message>
<xml_diff>
--- a/MATLAB/vehicle_data/zr25_data.xlsx
+++ b/MATLAB/vehicle_data/zr25_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bglen/Documents/github/Vehicle-Dynamics/MATLAB/vehicle_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1D509F9-E984-A344-98F3-05487CDDD2B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E2F4C7F-6A09-8C48-82D8-50649B593B7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="960" yWindow="500" windowWidth="16460" windowHeight="17500" xr2:uid="{3FBBEF13-1A9E-AE42-92D3-FE7D2663BCC6}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="13480" windowHeight="17500" xr2:uid="{3FBBEF13-1A9E-AE42-92D3-FE7D2663BCC6}"/>
   </bookViews>
   <sheets>
     <sheet name="parameters" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="151">
   <si>
     <t>Value</t>
   </si>
@@ -360,24 +360,6 @@
     <t>inertia of rim and tire</t>
   </si>
   <si>
-    <t>j_m</t>
-  </si>
-  <si>
-    <t>J_s1</t>
-  </si>
-  <si>
-    <t>J_1</t>
-  </si>
-  <si>
-    <t>J_2</t>
-  </si>
-  <si>
-    <t>J_s2</t>
-  </si>
-  <si>
-    <t>J_w</t>
-  </si>
-  <si>
     <t>inertia of gearbox input shaft (motor is the input shaft so this is zero)</t>
   </si>
   <si>
@@ -451,6 +433,60 @@
   </si>
   <si>
     <t>brake_pedal_motion_ratio</t>
+  </si>
+  <si>
+    <t>Jm</t>
+  </si>
+  <si>
+    <t>Js1</t>
+  </si>
+  <si>
+    <t>J1</t>
+  </si>
+  <si>
+    <t>J2</t>
+  </si>
+  <si>
+    <t>Js2</t>
+  </si>
+  <si>
+    <t>Jw</t>
+  </si>
+  <si>
+    <t>Dm</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>Dw</t>
+  </si>
+  <si>
+    <t>Ks1</t>
+  </si>
+  <si>
+    <t>Ks2</t>
+  </si>
+  <si>
+    <t>damping / viscous friction of motor</t>
+  </si>
+  <si>
+    <t>damping / viscous friction of input gear</t>
+  </si>
+  <si>
+    <t>damping / viscous friction of output gear</t>
+  </si>
+  <si>
+    <t>damping / viscous friction of wheel</t>
+  </si>
+  <si>
+    <t>rotational stiffness of input shaft</t>
+  </si>
+  <si>
+    <t>rotational stiffness of output shaft</t>
   </si>
 </sst>
 </file>
@@ -856,10 +892,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57AD0F8B-F3CF-1548-BE6B-192F596F87AA}">
-  <dimension ref="A1:E85"/>
+  <dimension ref="A1:E93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="D87" sqref="D87"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="109" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1104,7 +1140,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>108</v>
+        <v>133</v>
       </c>
       <c r="B25" s="1">
         <v>2.7399999999999999E-4</v>
@@ -1115,18 +1151,18 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>109</v>
+        <v>134</v>
       </c>
       <c r="B26" s="3">
         <v>0</v>
       </c>
       <c r="C26" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>110</v>
+        <v>135</v>
       </c>
       <c r="B27" s="3">
         <v>8.0000000000000004E-4</v>
@@ -1137,18 +1173,18 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>111</v>
+        <v>136</v>
       </c>
       <c r="B28" s="3">
         <v>0</v>
       </c>
       <c r="C28" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>112</v>
+        <v>137</v>
       </c>
       <c r="B29" s="3">
         <v>5.0000000000000001E-4</v>
@@ -1159,7 +1195,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>113</v>
+        <v>138</v>
       </c>
       <c r="B30" s="3">
         <v>3.0000000000000001E-3</v>
@@ -1169,561 +1205,633 @@
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" s="4"/>
+      <c r="A31" t="s">
+        <v>139</v>
+      </c>
+      <c r="B31" s="3">
+        <v>0</v>
+      </c>
+      <c r="C31" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>16</v>
+        <v>140</v>
       </c>
       <c r="B32" s="3">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="C32" t="s">
-        <v>49</v>
+        <v>146</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>17</v>
+        <v>141</v>
       </c>
       <c r="B33" s="3">
         <v>0</v>
       </c>
       <c r="C33" t="s">
-        <v>49</v>
+        <v>147</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>18</v>
+        <v>142</v>
       </c>
       <c r="B34" s="3">
-        <v>-2.5</v>
+        <v>0</v>
       </c>
       <c r="C34" t="s">
-        <v>50</v>
+        <v>148</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>19</v>
+        <v>143</v>
       </c>
       <c r="B35" s="3">
-        <v>-2.5</v>
+        <v>0</v>
       </c>
       <c r="C35" t="s">
-        <v>50</v>
+        <v>149</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>20</v>
+        <v>144</v>
       </c>
       <c r="B36" s="3">
-        <v>7.02</v>
+        <v>0</v>
       </c>
       <c r="C36" t="s">
-        <v>51</v>
+        <v>150</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>21</v>
-      </c>
-      <c r="B37" s="3">
-        <v>70</v>
-      </c>
-      <c r="C37" t="s">
-        <v>52</v>
-      </c>
+      <c r="B37" s="3"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>88</v>
-      </c>
-      <c r="B38" s="2">
-        <v>7.6176178298070302E-2</v>
-      </c>
-      <c r="C38" t="s">
-        <v>92</v>
-      </c>
+      <c r="B38" s="3"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>89</v>
-      </c>
-      <c r="B39" s="2">
-        <v>0.38417000000000001</v>
-      </c>
-      <c r="C39" t="s">
-        <v>93</v>
-      </c>
+      <c r="A39" s="4"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>97</v>
-      </c>
-      <c r="B40" s="2">
-        <v>0.38704984883732901</v>
+        <v>16</v>
+      </c>
+      <c r="B40" s="3">
+        <v>0.5</v>
       </c>
       <c r="C40" t="s">
-        <v>94</v>
+        <v>49</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>90</v>
-      </c>
-      <c r="B41" s="2">
-        <v>5.8772999999999999E-2</v>
+        <v>17</v>
+      </c>
+      <c r="B41" s="3">
+        <v>0</v>
       </c>
       <c r="C41" t="s">
-        <v>95</v>
+        <v>49</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>91</v>
-      </c>
-      <c r="B42" s="2">
-        <v>2.29E-2</v>
+        <v>18</v>
+      </c>
+      <c r="B42" s="3">
+        <v>-2.5</v>
       </c>
       <c r="C42" t="s">
-        <v>96</v>
+        <v>50</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>22</v>
-      </c>
-      <c r="B43" s="2">
-        <v>3.5000000000000003E-2</v>
+        <v>19</v>
+      </c>
+      <c r="B43" s="3">
+        <v>-2.5</v>
       </c>
       <c r="C43" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>23</v>
-      </c>
-      <c r="B44" s="2">
-        <v>0.05</v>
+        <v>20</v>
+      </c>
+      <c r="B44" s="3">
+        <v>7.02</v>
       </c>
       <c r="C44" t="s">
-        <v>54</v>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>21</v>
+      </c>
+      <c r="B45" s="3">
+        <v>70</v>
+      </c>
+      <c r="C45" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>24</v>
-      </c>
-      <c r="B46" s="3">
-        <v>1.5</v>
+        <v>88</v>
+      </c>
+      <c r="B46" s="2">
+        <v>7.6176178298070302E-2</v>
       </c>
       <c r="C46" t="s">
-        <v>55</v>
+        <v>92</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>25</v>
-      </c>
-      <c r="B47" s="3">
-        <v>0.2</v>
+        <v>89</v>
+      </c>
+      <c r="B47" s="2">
+        <v>0.38417000000000001</v>
       </c>
       <c r="C47" t="s">
-        <v>60</v>
+        <v>93</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>26</v>
-      </c>
-      <c r="B48" s="3">
-        <v>2</v>
+        <v>97</v>
+      </c>
+      <c r="B48" s="2">
+        <v>0.38704984883732901</v>
       </c>
       <c r="C48" t="s">
-        <v>61</v>
+        <v>94</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>27</v>
-      </c>
-      <c r="B49" s="3">
-        <v>0.45</v>
+        <v>90</v>
+      </c>
+      <c r="B49" s="2">
+        <v>5.8772999999999999E-2</v>
       </c>
       <c r="C49" t="s">
-        <v>56</v>
+        <v>95</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>28</v>
-      </c>
-      <c r="B50" s="1">
-        <v>11.4</v>
+        <v>91</v>
+      </c>
+      <c r="B50" s="2">
+        <v>2.29E-2</v>
       </c>
       <c r="C50" t="s">
-        <v>57</v>
+        <v>96</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>29</v>
-      </c>
-      <c r="B51" s="3">
-        <v>2.63</v>
+        <v>22</v>
+      </c>
+      <c r="B51" s="2">
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="C51" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>30</v>
-      </c>
-      <c r="B52" s="3">
-        <v>0.45500000000000002</v>
+        <v>23</v>
+      </c>
+      <c r="B52" s="2">
+        <v>0.05</v>
       </c>
       <c r="C52" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
-        <v>31</v>
-      </c>
-      <c r="B53" s="3">
-        <v>31</v>
-      </c>
-      <c r="C53" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B54" s="3">
-        <v>2.59</v>
+        <v>1.5</v>
       </c>
       <c r="C54" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="B55" s="3">
-        <v>0.27600000000000002</v>
+        <v>0.2</v>
       </c>
       <c r="C55" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A56" s="4"/>
+      <c r="A56" t="s">
+        <v>26</v>
+      </c>
+      <c r="B56" s="3">
+        <v>2</v>
+      </c>
+      <c r="C56" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B57" s="3">
-        <v>5.5E-2</v>
+        <v>0.45</v>
       </c>
       <c r="C57" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
+        <v>28</v>
+      </c>
+      <c r="B58" s="1">
+        <v>11.4</v>
+      </c>
+      <c r="C58" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>29</v>
+      </c>
+      <c r="B59" s="3">
+        <v>2.63</v>
+      </c>
+      <c r="C59" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>30</v>
+      </c>
+      <c r="B60" s="3">
+        <v>0.45500000000000002</v>
+      </c>
+      <c r="C60" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>31</v>
+      </c>
+      <c r="B61" s="3">
+        <v>31</v>
+      </c>
+      <c r="C61" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>32</v>
+      </c>
+      <c r="B62" s="3">
+        <v>2.59</v>
+      </c>
+      <c r="C62" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>33</v>
+      </c>
+      <c r="B63" s="3">
+        <v>0.27600000000000002</v>
+      </c>
+      <c r="C63" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A64" s="4"/>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>34</v>
+      </c>
+      <c r="B65" s="3">
+        <v>5.5E-2</v>
+      </c>
+      <c r="C65" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
         <v>35</v>
       </c>
-      <c r="B58" s="2">
+      <c r="B66" s="2">
         <f xml:space="preserve"> 45 * 1000</f>
         <v>45000</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C66" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
         <v>36</v>
       </c>
-      <c r="B59" s="2">
+      <c r="B67" s="2">
         <f xml:space="preserve"> 35 * 1000</f>
         <v>35000</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C67" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
         <v>37</v>
       </c>
-      <c r="B60" s="3">
+      <c r="B68" s="3">
         <v>2</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C68" t="s">
         <v>67</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
-        <v>38</v>
-      </c>
-      <c r="B61" s="3">
-        <v>160.23070000000001</v>
-      </c>
-      <c r="C61" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
-        <v>39</v>
-      </c>
-      <c r="B62" s="2">
-        <v>1.0009999999999999</v>
-      </c>
-      <c r="C62" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
-        <v>40</v>
-      </c>
-      <c r="B63" s="2">
-        <v>1.006</v>
-      </c>
-      <c r="C63" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
-        <v>41</v>
-      </c>
-      <c r="B64" s="3">
-        <v>1</v>
-      </c>
-      <c r="C64" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
-        <v>42</v>
-      </c>
-      <c r="B65" s="3">
-        <v>0.158</v>
-      </c>
-      <c r="C65" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
-        <v>43</v>
-      </c>
-      <c r="B66" s="2">
-        <v>3.4</v>
-      </c>
-      <c r="C66" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
-        <v>44</v>
-      </c>
-      <c r="B67" s="2">
-        <v>3.7</v>
-      </c>
-      <c r="C67" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>102</v>
-      </c>
-      <c r="B69" s="2">
-        <v>0.1</v>
+        <v>38</v>
+      </c>
+      <c r="B69" s="3">
+        <v>160.23070000000001</v>
       </c>
       <c r="C69" t="s">
-        <v>101</v>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>39</v>
+      </c>
+      <c r="B70" s="2">
+        <v>1.0009999999999999</v>
+      </c>
+      <c r="C70" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>116</v>
+        <v>40</v>
       </c>
       <c r="B71" s="2">
-        <v>1.2999999999999999E-2</v>
+        <v>1.006</v>
       </c>
       <c r="C71" t="s">
-        <v>128</v>
+        <v>69</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>117</v>
-      </c>
-      <c r="B72" s="2">
-        <v>1.2999999999999999E-2</v>
+        <v>41</v>
+      </c>
+      <c r="B72" s="3">
+        <v>1</v>
       </c>
       <c r="C72" t="s">
-        <v>128</v>
+        <v>70</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>127</v>
-      </c>
-      <c r="B73" s="2">
-        <v>2</v>
+        <v>42</v>
+      </c>
+      <c r="B73" s="3">
+        <v>0.158</v>
       </c>
       <c r="C73" t="s">
-        <v>122</v>
+        <v>70</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>118</v>
+        <v>43</v>
       </c>
       <c r="B74" s="2">
-        <v>2</v>
+        <v>3.4</v>
       </c>
       <c r="C74" t="s">
-        <v>122</v>
+        <v>71</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>119</v>
+        <v>44</v>
       </c>
       <c r="B75" s="2">
-        <v>0.5</v>
+        <v>3.7</v>
       </c>
       <c r="C75" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A76" t="s">
-        <v>120</v>
-      </c>
-      <c r="B76" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="C76" t="s">
-        <v>122</v>
+        <v>72</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>121</v>
+        <v>102</v>
       </c>
       <c r="B77" s="2">
-        <v>667.23</v>
+        <v>0.1</v>
       </c>
       <c r="C77" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A78" t="s">
-        <v>123</v>
-      </c>
-      <c r="B78" s="2">
-        <v>0.13</v>
-      </c>
-      <c r="C78" t="s">
-        <v>136</v>
+        <v>101</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>124</v>
+        <v>110</v>
       </c>
       <c r="B79" s="2">
-        <v>0.13</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="C79" t="s">
-        <v>136</v>
+        <v>122</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>125</v>
+        <v>111</v>
       </c>
       <c r="B80" s="2">
-        <v>2.5000000000000001E-2</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="C80" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="B81" s="2">
-        <v>2.5000000000000001E-2</v>
+        <v>2</v>
       </c>
       <c r="C81" t="s">
-        <v>135</v>
+        <v>116</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
       <c r="B82" s="2">
-        <v>1.6E-2</v>
+        <v>2</v>
       </c>
       <c r="C82" t="s">
-        <v>133</v>
+        <v>116</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>131</v>
+        <v>113</v>
       </c>
       <c r="B83" s="2">
-        <v>2.4E-2</v>
+        <v>0.5</v>
       </c>
       <c r="C83" t="s">
-        <v>134</v>
+        <v>116</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>132</v>
+        <v>114</v>
       </c>
       <c r="B84" s="2">
-        <v>0.51519999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="C84" t="s">
-        <v>137</v>
+        <v>116</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>138</v>
+        <v>115</v>
       </c>
       <c r="B85" s="2">
+        <v>667.23</v>
+      </c>
+      <c r="C85" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>117</v>
+      </c>
+      <c r="B86" s="2">
+        <v>0.13</v>
+      </c>
+      <c r="C86" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>118</v>
+      </c>
+      <c r="B87" s="2">
+        <v>0.13</v>
+      </c>
+      <c r="C87" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>119</v>
+      </c>
+      <c r="B88" s="2">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="C88" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>120</v>
+      </c>
+      <c r="B89" s="2">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="C89" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>124</v>
+      </c>
+      <c r="B90" s="2">
+        <v>1.6E-2</v>
+      </c>
+      <c r="C90" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>125</v>
+      </c>
+      <c r="B91" s="2">
+        <v>2.4E-2</v>
+      </c>
+      <c r="C91" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>126</v>
+      </c>
+      <c r="B92" s="2">
+        <v>0.51519999999999999</v>
+      </c>
+      <c r="C92" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>132</v>
+      </c>
+      <c r="B93" s="2">
         <v>3.77</v>
       </c>
-      <c r="C85" t="s">
-        <v>122</v>
+      <c r="C93" t="s">
+        <v>116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added simple longitudinal vehicle model to verify wheel dynamics
</commit_message>
<xml_diff>
--- a/MATLAB/vehicle_data/zr25_data.xlsx
+++ b/MATLAB/vehicle_data/zr25_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bglen/Documents/github/Vehicle-Dynamics/MATLAB/vehicle_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE555E40-9553-3A4F-8F22-15073653F8D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F826283-E368-DB41-AD7E-F7A3DCFC33A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{3FBBEF13-1A9E-AE42-92D3-FE7D2663BCC6}"/>
+    <workbookView xWindow="2560" yWindow="500" windowWidth="26240" windowHeight="17500" xr2:uid="{3FBBEF13-1A9E-AE42-92D3-FE7D2663BCC6}"/>
   </bookViews>
   <sheets>
     <sheet name="parameters" sheetId="1" r:id="rId1"/>
@@ -895,7 +895,7 @@
   <dimension ref="A1:E91"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A23" zoomScale="223" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1143,7 +1143,7 @@
         <v>129</v>
       </c>
       <c r="B25" s="1">
-        <v>9.9999999999999995E-8</v>
+        <v>2.7399999999999999E-4</v>
       </c>
       <c r="C25" t="s">
         <v>147</v>
@@ -1165,7 +1165,7 @@
         <v>131</v>
       </c>
       <c r="B27" s="1">
-        <v>9.9999999999999995E-8</v>
+        <v>3.9389999999999998E-4</v>
       </c>
       <c r="C27" t="s">
         <v>148</v>
@@ -1198,7 +1198,7 @@
         <v>134</v>
       </c>
       <c r="B30" s="1">
-        <v>2.9999999999999997E-4</v>
+        <v>0.3</v>
       </c>
       <c r="C30" t="s">
         <v>149</v>

</xml_diff>